<commit_message>
Update araç web site mock-up.xlsx
</commit_message>
<xml_diff>
--- a/araç web site mock-up.xlsx
+++ b/araç web site mock-up.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faruk\OneDrive\Belgeler\GitHub\devops-dersler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700BF927-4DFA-4EB1-8247-EE884BC57D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF87CAD-B235-4E1E-9A34-690EF4F9FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5CFAE102-0AFE-4949-B11C-41DB58945217}"/>
   </bookViews>
@@ -4401,13 +4401,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:colOff>1495425</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -4424,8 +4424,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7648575" y="228600"/>
-          <a:ext cx="1438275" cy="447675"/>
+          <a:off x="7686675" y="266700"/>
+          <a:ext cx="1438275" cy="523875"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4537,15 +4537,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2038350</xdr:colOff>
+      <xdr:colOff>2085975</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4560,8 +4560,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3648075" y="342900"/>
-          <a:ext cx="1695450" cy="504825"/>
+          <a:off x="3695700" y="400050"/>
+          <a:ext cx="1695450" cy="619125"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4608,15 +4608,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:colOff>1838325</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4631,8 +4631,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3724275" y="990600"/>
-          <a:ext cx="1438275" cy="447675"/>
+          <a:off x="3705225" y="1104900"/>
+          <a:ext cx="1438275" cy="523875"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4676,15 +4676,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>2047875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4699,8 +4699,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3638549" y="1666875"/>
-          <a:ext cx="1647826" cy="447675"/>
+          <a:off x="3705224" y="1790700"/>
+          <a:ext cx="1647826" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5748,7 +5748,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>